<commit_message>
biopsykit.io.load_time_log(): added "phase" to column name of time log dataframe
</commit_message>
<xml_diff>
--- a/tests/test_data/time_log.xlsx
+++ b/tests/test_data/time_log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/BioPsyKit/tests/data/test_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/PhD/Projects/BioPsyKit/tests/test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE2A005E-B739-B24E-A56D-4CA1F788EFDF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F21E3D-AEE9-B048-9FDF-76225B7D1E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16360"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="time_log copy" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -890,10 +890,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>